<commit_message>
fixed accidental error in example data
</commit_message>
<xml_diff>
--- a/ExampleData.xlsx
+++ b/ExampleData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\VSCode\PythonScripts\corining_app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEEC4A3F-A0A1-4534-A91E-479EDA2BE0F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C216FAD-3AC4-42BA-BEAC-65CE4F80177A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="15">
   <si>
     <t>Reference Configuration</t>
   </si>
@@ -1839,17 +1839,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A42"/>
     <mergeCell ref="A93:A102"/>
     <mergeCell ref="A43:A52"/>
     <mergeCell ref="A53:A62"/>
     <mergeCell ref="A63:A72"/>
     <mergeCell ref="A73:A82"/>
     <mergeCell ref="A83:A92"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A42"/>
   </mergeCells>
   <conditionalFormatting sqref="C13:D22">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="notEqual">
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:D102"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="M81" sqref="M81"/>
+      <selection activeCell="I101" sqref="I101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3117,8 +3117,8 @@
       <c r="B101">
         <v>9</v>
       </c>
-      <c r="C101" s="1">
-        <v>1</v>
+      <c r="C101" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>5</v>
@@ -3132,23 +3132,23 @@
       <c r="C102" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D102" s="1">
-        <v>1</v>
+      <c r="D102" s="1" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A42"/>
     <mergeCell ref="A93:A102"/>
     <mergeCell ref="A43:A52"/>
     <mergeCell ref="A53:A62"/>
     <mergeCell ref="A63:A72"/>
     <mergeCell ref="A73:A82"/>
     <mergeCell ref="A83:A92"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A42"/>
   </mergeCells>
   <conditionalFormatting sqref="C13:D22">
     <cfRule type="cellIs" dxfId="14" priority="1" operator="notEqual">
@@ -4437,17 +4437,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A42"/>
     <mergeCell ref="A93:A102"/>
     <mergeCell ref="A43:A52"/>
     <mergeCell ref="A53:A62"/>
     <mergeCell ref="A63:A72"/>
     <mergeCell ref="A73:A82"/>
     <mergeCell ref="A83:A92"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A42"/>
   </mergeCells>
   <conditionalFormatting sqref="C13:D22">
     <cfRule type="cellIs" dxfId="9" priority="1" operator="notEqual">
@@ -5736,17 +5736,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="A3:A12"/>
-    <mergeCell ref="A13:A22"/>
-    <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A42"/>
     <mergeCell ref="A93:A102"/>
     <mergeCell ref="A43:A52"/>
     <mergeCell ref="A53:A62"/>
     <mergeCell ref="A63:A72"/>
     <mergeCell ref="A73:A82"/>
     <mergeCell ref="A83:A92"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="A3:A12"/>
+    <mergeCell ref="A13:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A42"/>
   </mergeCells>
   <conditionalFormatting sqref="C13:D22">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="notEqual">

</xml_diff>